<commit_message>
thêm báo cáo chi phí bán hàng
</commit_message>
<xml_diff>
--- a/Project/Database/dulieumau.xlsx
+++ b/Project/Database/dulieumau.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Vinh\HOC TAP\UIT\Phan Tich Thiet Ke\DoAn\PhanTichThietKe\Project\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7635" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="BILL" sheetId="1" r:id="rId1"/>
@@ -184,45 +184,30 @@
     <t>complete</t>
   </si>
   <si>
-    <t>PR00001</t>
-  </si>
-  <si>
     <t>USB SanDisk Cruzer CZ71 16GB</t>
   </si>
   <si>
     <t>Picture\Product\000001.png</t>
   </si>
   <si>
-    <t>PR00002</t>
-  </si>
-  <si>
     <t>Laptop Asus F454LA-WX390D (Free Dos)</t>
   </si>
   <si>
     <t>Picture\Product\000002.png</t>
   </si>
   <si>
-    <t>PR00003</t>
-  </si>
-  <si>
     <t>Laptop Dell N5558-DPXRD4 (Win 8.1)</t>
   </si>
   <si>
     <t>Picture\Product\000003.png</t>
   </si>
   <si>
-    <t>PR00004</t>
-  </si>
-  <si>
     <t>Thẻ Nhớ Micro SD Ultra Sandisk 32GB Class 10 - 48MB/s</t>
   </si>
   <si>
     <t>Picture\Product\000004.png</t>
   </si>
   <si>
-    <t>PR00005</t>
-  </si>
-  <si>
     <t>Màn Hình Dell U2414H 24"</t>
   </si>
   <si>
@@ -482,6 +467,21 @@
   </si>
   <si>
     <t>47 Nguyễn Tư Giản, phường 12, Gò Vấp, Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>PR000001</t>
+  </si>
+  <si>
+    <t>PR000002</t>
+  </si>
+  <si>
+    <t>PR000003</t>
+  </si>
+  <si>
+    <t>PR000004</t>
+  </si>
+  <si>
+    <t>PR000005</t>
   </si>
 </sst>
 </file>
@@ -826,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,7 +1840,7 @@
   <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,16 +1855,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D2" s="3">
         <v>6755676</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="3">
         <v>100000</v>
@@ -1878,16 +1878,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>142</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3">
         <v>6755676</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F3" s="3">
         <v>7000000</v>
@@ -1901,16 +1901,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>6755676</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F4" s="3">
         <v>14000000</v>
@@ -1924,16 +1924,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3">
         <v>6755676</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3">
         <v>200000</v>
@@ -1947,16 +1947,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3">
         <v>6755676</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F6" s="3">
         <v>5200000</v>
@@ -1970,16 +1970,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3">
         <v>12345679</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F7" s="3">
         <v>3000000</v>
@@ -1993,16 +1993,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3">
         <v>12345679</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F8" s="3">
         <v>3000000</v>
@@ -2016,16 +2016,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3">
         <v>12345679</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F9" s="3">
         <v>1500000</v>
@@ -2039,16 +2039,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D10" s="3">
         <v>12345679</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F10" s="3">
         <v>10000000</v>
@@ -2062,16 +2062,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D11" s="3">
         <v>12345679</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F11" s="3">
         <v>4000000</v>
@@ -2085,16 +2085,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D12" s="3">
         <v>12345679</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F12" s="3">
         <v>20000000</v>
@@ -2108,16 +2108,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D13" s="3">
         <v>12345679</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F13" s="3">
         <v>20000000</v>
@@ -2131,16 +2131,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D14" s="3">
         <v>12345679</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F14" s="3">
         <v>90000</v>
@@ -2154,16 +2154,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D15" s="3">
         <v>12345679</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F15" s="3">
         <v>110000</v>
@@ -2181,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2198,10 +2198,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,10 +2212,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2226,10 +2226,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2240,10 +2240,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,10 +2254,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,10 +2268,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,10 +2282,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,10 +2296,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2310,10 +2310,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2324,10 +2324,10 @@
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,10 +2338,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2352,10 +2352,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2366,10 +2366,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2380,10 +2380,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,10 +2394,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2408,10 +2408,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2422,10 +2422,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2436,10 +2436,10 @@
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2450,10 +2450,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2464,10 +2464,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2478,10 +2478,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2492,10 +2492,10 @@
         <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2506,10 +2506,10 @@
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2520,10 +2520,10 @@
         <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2534,10 +2534,10 @@
         <v>9</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2548,10 +2548,10 @@
         <v>9</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2562,10 +2562,10 @@
         <v>9</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2576,10 +2576,10 @@
         <v>10</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2590,10 +2590,10 @@
         <v>10</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2604,10 +2604,10 @@
         <v>10</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2618,10 +2618,10 @@
         <v>11</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2632,10 +2632,10 @@
         <v>11</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2646,10 +2646,10 @@
         <v>11</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2660,10 +2660,10 @@
         <v>12</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2674,10 +2674,10 @@
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2688,10 +2688,10 @@
         <v>12</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2702,10 +2702,10 @@
         <v>13</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2716,10 +2716,10 @@
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2730,10 +2730,10 @@
         <v>13</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2744,10 +2744,10 @@
         <v>14</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2758,10 +2758,10 @@
         <v>14</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2772,10 +2772,10 @@
         <v>14</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2854,10 +2854,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D2" s="3">
         <v>91</v>
@@ -2866,16 +2866,16 @@
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H2" s="3">
         <v>123456789</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J2" s="4">
         <v>32874</v>
@@ -2889,10 +2889,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3">
         <v>92</v>
@@ -2901,16 +2901,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H3" s="3">
         <v>123456789</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J3" s="4">
         <v>32874</v>
@@ -2933,7 +2933,7 @@
   <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,16 +2949,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2966,16 +2966,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2983,16 +2983,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3000,16 +3000,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3017,16 +3017,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3034,16 +3034,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3051,16 +3051,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3068,16 +3068,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>